<commit_message>
Updated backlog to show CC and CO completed. CS in progress.
</commit_message>
<xml_diff>
--- a/P10/Scrum_MICE_Sprint_4.xlsx
+++ b/P10/Scrum_MICE_Sprint_4.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="210">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -662,6 +662,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create a new container.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Work</t>
   </si>
   <si>
     <t xml:space="preserve">--&gt; Add tasks to complete each feature for this sprint</t>
@@ -885,7 +888,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1046,10 +1049,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1127,7 +1126,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1173,10 +1172,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822405395279131"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.884351192706382"/>
-          <c:h val="0.63565305093293"/>
+          <c:x val="0.0822456753887466"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.884281521263973"/>
+          <c:h val="0.635607111335267"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1285,11 +1284,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96877657"/>
-        <c:axId val="40361249"/>
+        <c:axId val="80553179"/>
+        <c:axId val="20081744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96877657"/>
+        <c:axId val="80553179"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1356,12 +1355,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40361249"/>
+        <c:crossAx val="20081744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40361249"/>
+        <c:axId val="20081744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1436,7 +1435,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96877657"/>
+        <c:crossAx val="80553179"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1456,14 +1455,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1591,11 +1590,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73976579"/>
-        <c:axId val="14517215"/>
+        <c:axId val="17383742"/>
+        <c:axId val="49903217"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73976579"/>
+        <c:axId val="17383742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1660,7 +1659,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14517215"/>
+        <c:crossAx val="49903217"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1668,7 +1667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14517215"/>
+        <c:axId val="49903217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,7 +1741,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73976579"/>
+        <c:crossAx val="17383742"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1762,14 +1761,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1897,11 +1896,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34125249"/>
-        <c:axId val="57639660"/>
+        <c:axId val="49383222"/>
+        <c:axId val="42684288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34125249"/>
+        <c:axId val="49383222"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,7 +1965,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57639660"/>
+        <c:crossAx val="42684288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1974,7 +1973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57639660"/>
+        <c:axId val="42684288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2048,7 +2047,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34125249"/>
+        <c:crossAx val="49383222"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2068,14 +2067,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2203,11 +2202,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="13353750"/>
-        <c:axId val="46920433"/>
+        <c:axId val="78726740"/>
+        <c:axId val="19421657"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13353750"/>
+        <c:axId val="78726740"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2271,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46920433"/>
+        <c:crossAx val="19421657"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2280,7 +2279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46920433"/>
+        <c:axId val="19421657"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2353,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13353750"/>
+        <c:crossAx val="78726740"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2374,14 +2373,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2494,7 +2493,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,11 +2508,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57348697"/>
-        <c:axId val="3397386"/>
+        <c:axId val="52563442"/>
+        <c:axId val="71535695"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57348697"/>
+        <c:axId val="52563442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2578,7 +2577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3397386"/>
+        <c:crossAx val="71535695"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2586,7 +2585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3397386"/>
+        <c:axId val="71535695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,7 +2659,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57348697"/>
+        <c:crossAx val="52563442"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2680,14 +2679,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2815,11 +2814,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81528983"/>
-        <c:axId val="53187718"/>
+        <c:axId val="69541736"/>
+        <c:axId val="12256632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81528983"/>
+        <c:axId val="69541736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2884,7 +2883,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53187718"/>
+        <c:crossAx val="12256632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2892,7 +2891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53187718"/>
+        <c:axId val="12256632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2966,7 +2965,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81528983"/>
+        <c:crossAx val="69541736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2986,14 +2985,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3121,11 +3120,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="3081335"/>
-        <c:axId val="55082044"/>
+        <c:axId val="21803028"/>
+        <c:axId val="66519995"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="3081335"/>
+        <c:axId val="21803028"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3190,7 +3189,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55082044"/>
+        <c:crossAx val="66519995"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3198,7 +3197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55082044"/>
+        <c:axId val="66519995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3272,7 +3271,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3081335"/>
+        <c:crossAx val="21803028"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3292,7 +3291,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3310,9 +3309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3202200</xdr:colOff>
+      <xdr:colOff>3201840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3320,8 +3319,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9118080" y="268200"/>
-        <a:ext cx="5764680" cy="2855160"/>
+        <a:off x="9116280" y="268200"/>
+        <a:ext cx="5764320" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3345,9 +3344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3355,8 +3354,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3380,9 +3379,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3390,8 +3389,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3415,9 +3414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3425,8 +3424,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3450,9 +3449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3460,8 +3459,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3485,9 +3484,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3495,8 +3494,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3520,9 +3519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3530,8 +3529,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3561,11 +3560,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.71"/>
@@ -5590,7 +5589,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6572,7 +6571,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7545,7 +7544,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8533,10 +8532,10 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8733,11 +8732,11 @@
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="27" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -8792,11 +8791,11 @@
       <c r="B18" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="23" t="s">
         <v>78</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8806,7 +8805,7 @@
       <c r="B19" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="23" t="s">
         <v>82</v>
       </c>
       <c r="E19" s="37" t="s">
@@ -9514,7 +9513,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9755,8 +9754,8 @@
         <v>1</v>
       </c>
       <c r="B17" s="38"/>
-      <c r="D17" s="41" t="s">
-        <v>206</v>
+      <c r="D17" s="40" t="s">
+        <v>207</v>
       </c>
       <c r="E17" s="39"/>
     </row>
@@ -10473,7 +10472,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10490,7 +10489,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>2</v>
@@ -10686,7 +10685,7 @@
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
@@ -10716,8 +10715,8 @@
         <v>1</v>
       </c>
       <c r="B17" s="38"/>
-      <c r="D17" s="41" t="s">
-        <v>206</v>
+      <c r="D17" s="40" t="s">
+        <v>207</v>
       </c>
       <c r="E17" s="39"/>
     </row>

</xml_diff>